<commit_message>
adding unmarshaller for json-response
</commit_message>
<xml_diff>
--- a/punkteverteilung.xlsx
+++ b/punkteverteilung.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="198"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="17565" windowHeight="8085" tabRatio="198"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -213,8 +214,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -240,7 +241,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -256,12 +257,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="22"/>
-        <bgColor indexed="31"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
         <bgColor indexed="31"/>
       </patternFill>
     </fill>
@@ -296,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -326,22 +321,19 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -427,7 +419,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -501,7 +493,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -536,7 +527,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -712,14 +702,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="11.5703125" style="1"/>
     <col min="2" max="2" width="39.7109375" style="1" customWidth="1"/>
@@ -728,7 +718,7 @@
     <col min="5" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -742,8 +732,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
+    <row r="2" spans="1:4" ht="25.5">
+      <c r="A2" s="15" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -755,8 +745,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="17"/>
+    <row r="3" spans="1:4">
+      <c r="A3" s="16"/>
       <c r="B3" s="8" t="s">
         <v>6</v>
       </c>
@@ -765,8 +755,8 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="17"/>
+    <row r="4" spans="1:4">
+      <c r="A4" s="16"/>
       <c r="B4" s="8" t="s">
         <v>7</v>
       </c>
@@ -775,8 +765,8 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="17"/>
+    <row r="5" spans="1:4" ht="25.5">
+      <c r="A5" s="16"/>
       <c r="B5" s="8" t="s">
         <v>8</v>
       </c>
@@ -785,8 +775,8 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="17"/>
+    <row r="6" spans="1:4" ht="38.25">
+      <c r="A6" s="16"/>
       <c r="B6" s="8" t="s">
         <v>9</v>
       </c>
@@ -795,8 +785,8 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="17"/>
+    <row r="7" spans="1:4" ht="25.5">
+      <c r="A7" s="16"/>
       <c r="B7" s="8" t="s">
         <v>10</v>
       </c>
@@ -805,8 +795,8 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="18"/>
+    <row r="8" spans="1:4" ht="38.25">
+      <c r="A8" s="17"/>
       <c r="B8" s="8" t="s">
         <v>11</v>
       </c>
@@ -815,8 +805,8 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A9" s="13" t="s">
+    <row r="9" spans="1:4" ht="25.5">
+      <c r="A9" s="15" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -830,8 +820,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A10" s="17"/>
+    <row r="10" spans="1:4" ht="25.5">
+      <c r="A10" s="16"/>
       <c r="B10" s="8" t="s">
         <v>14</v>
       </c>
@@ -840,8 +830,8 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="14"/>
+    <row r="11" spans="1:4" ht="25.5">
+      <c r="A11" s="13"/>
       <c r="B11" s="8" t="s">
         <v>15</v>
       </c>
@@ -850,8 +840,8 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="15"/>
+    <row r="12" spans="1:4" ht="38.25">
+      <c r="A12" s="14"/>
       <c r="B12" s="8" t="s">
         <v>16</v>
       </c>
@@ -860,8 +850,8 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A13" s="16" t="s">
+    <row r="13" spans="1:4" ht="51">
+      <c r="A13" s="15" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -875,8 +865,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A14" s="17"/>
+    <row r="14" spans="1:4" ht="25.5">
+      <c r="A14" s="16"/>
       <c r="B14" s="8" t="s">
         <v>19</v>
       </c>
@@ -885,8 +875,8 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A15" s="17"/>
+    <row r="15" spans="1:4" ht="25.5">
+      <c r="A15" s="16"/>
       <c r="B15" s="8" t="s">
         <v>20</v>
       </c>
@@ -895,8 +885,8 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A16" s="17"/>
+    <row r="16" spans="1:4" ht="25.5">
+      <c r="A16" s="16"/>
       <c r="B16" s="8" t="s">
         <v>21</v>
       </c>
@@ -905,8 +895,8 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="17"/>
+    <row r="17" spans="1:4" ht="25.5">
+      <c r="A17" s="16"/>
       <c r="B17" s="8" t="s">
         <v>22</v>
       </c>
@@ -915,8 +905,8 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A18" s="17"/>
+    <row r="18" spans="1:4" ht="25.5">
+      <c r="A18" s="16"/>
       <c r="B18" s="8" t="s">
         <v>23</v>
       </c>
@@ -925,8 +915,8 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A19" s="17"/>
+    <row r="19" spans="1:4" ht="38.25">
+      <c r="A19" s="16"/>
       <c r="B19" s="8" t="s">
         <v>24</v>
       </c>
@@ -935,8 +925,8 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A20" s="14"/>
+    <row r="20" spans="1:4" ht="38.25">
+      <c r="A20" s="16"/>
       <c r="B20" s="8" t="s">
         <v>25</v>
       </c>
@@ -945,8 +935,8 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="14"/>
+    <row r="21" spans="1:4">
+      <c r="A21" s="16"/>
       <c r="B21" s="8" t="s">
         <v>26</v>
       </c>
@@ -955,8 +945,8 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A22" s="17"/>
+    <row r="22" spans="1:4" ht="25.5">
+      <c r="A22" s="16"/>
       <c r="B22" s="8" t="s">
         <v>27</v>
       </c>
@@ -965,8 +955,8 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A23" s="17"/>
+    <row r="23" spans="1:4" ht="25.5">
+      <c r="A23" s="16"/>
       <c r="B23" s="8" t="s">
         <v>28</v>
       </c>
@@ -975,8 +965,8 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A24" s="18"/>
+    <row r="24" spans="1:4" ht="38.25">
+      <c r="A24" s="17"/>
       <c r="B24" s="8" t="s">
         <v>29</v>
       </c>
@@ -985,8 +975,8 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A25" s="16" t="s">
+    <row r="25" spans="1:4" ht="38.25">
+      <c r="A25" s="15" t="s">
         <v>30</v>
       </c>
       <c r="B25" s="5" t="s">
@@ -1000,16 +990,16 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A26" s="17"/>
+    <row r="26" spans="1:4" ht="25.5">
+      <c r="A26" s="16"/>
       <c r="B26" s="8" t="s">
         <v>32</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="17"/>
+    <row r="27" spans="1:4">
+      <c r="A27" s="16"/>
       <c r="B27" s="8" t="s">
         <v>33</v>
       </c>
@@ -1018,8 +1008,8 @@
       </c>
       <c r="D27" s="7"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="17"/>
+    <row r="28" spans="1:4">
+      <c r="A28" s="16"/>
       <c r="B28" s="8" t="s">
         <v>34</v>
       </c>
@@ -1028,8 +1018,8 @@
       </c>
       <c r="D28" s="7"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="17"/>
+    <row r="29" spans="1:4">
+      <c r="A29" s="16"/>
       <c r="B29" s="8" t="s">
         <v>35</v>
       </c>
@@ -1038,8 +1028,8 @@
       </c>
       <c r="D29" s="7"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="17"/>
+    <row r="30" spans="1:4">
+      <c r="A30" s="16"/>
       <c r="B30" s="8" t="s">
         <v>36</v>
       </c>
@@ -1048,8 +1038,8 @@
       </c>
       <c r="D30" s="7"/>
     </row>
-    <row r="31" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A31" s="17"/>
+    <row r="31" spans="1:4" ht="38.25">
+      <c r="A31" s="16"/>
       <c r="B31" s="8" t="s">
         <v>37</v>
       </c>
@@ -1058,8 +1048,8 @@
       </c>
       <c r="D31" s="7"/>
     </row>
-    <row r="32" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A32" s="17"/>
+    <row r="32" spans="1:4" ht="51">
+      <c r="A32" s="16"/>
       <c r="B32" s="8" t="s">
         <v>38</v>
       </c>
@@ -1068,8 +1058,8 @@
       </c>
       <c r="D32" s="7"/>
     </row>
-    <row r="33" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A33" s="17"/>
+    <row r="33" spans="1:4" ht="51">
+      <c r="A33" s="16"/>
       <c r="B33" s="8" t="s">
         <v>39</v>
       </c>
@@ -1078,8 +1068,8 @@
       </c>
       <c r="D33" s="7"/>
     </row>
-    <row r="34" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A34" s="17"/>
+    <row r="34" spans="1:4" ht="51">
+      <c r="A34" s="16"/>
       <c r="B34" s="8" t="s">
         <v>40</v>
       </c>
@@ -1088,8 +1078,8 @@
       </c>
       <c r="D34" s="7"/>
     </row>
-    <row r="35" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A35" s="17"/>
+    <row r="35" spans="1:4" ht="51">
+      <c r="A35" s="16"/>
       <c r="B35" s="8" t="s">
         <v>41</v>
       </c>
@@ -1098,8 +1088,8 @@
       </c>
       <c r="D35" s="7"/>
     </row>
-    <row r="36" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A36" s="18"/>
+    <row r="36" spans="1:4" ht="38.25">
+      <c r="A36" s="17"/>
       <c r="B36" s="8" t="s">
         <v>42</v>
       </c>
@@ -1108,8 +1098,8 @@
       </c>
       <c r="D36" s="7"/>
     </row>
-    <row r="37" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A37" s="16" t="s">
+    <row r="37" spans="1:4" ht="25.5">
+      <c r="A37" s="15" t="s">
         <v>43</v>
       </c>
       <c r="B37" s="5" t="s">
@@ -1123,16 +1113,16 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A38" s="17"/>
+    <row r="38" spans="1:4" ht="25.5">
+      <c r="A38" s="16"/>
       <c r="B38" s="8" t="s">
         <v>45</v>
       </c>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="17"/>
+    <row r="39" spans="1:4">
+      <c r="A39" s="16"/>
       <c r="B39" s="8" t="s">
         <v>46</v>
       </c>
@@ -1141,8 +1131,8 @@
       </c>
       <c r="D39" s="7"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="17"/>
+    <row r="40" spans="1:4">
+      <c r="A40" s="16"/>
       <c r="B40" s="8" t="s">
         <v>47</v>
       </c>
@@ -1151,8 +1141,8 @@
       </c>
       <c r="D40" s="7"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="17"/>
+    <row r="41" spans="1:4">
+      <c r="A41" s="16"/>
       <c r="B41" s="8" t="s">
         <v>48</v>
       </c>
@@ -1161,8 +1151,8 @@
       </c>
       <c r="D41" s="7"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="17"/>
+    <row r="42" spans="1:4">
+      <c r="A42" s="16"/>
       <c r="B42" s="8" t="s">
         <v>49</v>
       </c>
@@ -1171,8 +1161,8 @@
       </c>
       <c r="D42" s="7"/>
     </row>
-    <row r="43" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A43" s="17"/>
+    <row r="43" spans="1:4" ht="51">
+      <c r="A43" s="16"/>
       <c r="B43" s="8" t="s">
         <v>50</v>
       </c>
@@ -1181,8 +1171,8 @@
       </c>
       <c r="D43" s="7"/>
     </row>
-    <row r="44" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A44" s="18"/>
+    <row r="44" spans="1:4" ht="25.5">
+      <c r="A44" s="17"/>
       <c r="B44" s="8" t="s">
         <v>51</v>
       </c>
@@ -1191,8 +1181,8 @@
       </c>
       <c r="D44" s="7"/>
     </row>
-    <row r="45" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A45" s="16" t="s">
+    <row r="45" spans="1:4" ht="38.25">
+      <c r="A45" s="15" t="s">
         <v>52</v>
       </c>
       <c r="B45" s="5" t="s">
@@ -1206,8 +1196,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A46" s="17"/>
+    <row r="46" spans="1:4" ht="25.5">
+      <c r="A46" s="16"/>
       <c r="B46" s="8" t="s">
         <v>54</v>
       </c>
@@ -1216,8 +1206,8 @@
       </c>
       <c r="D46" s="7"/>
     </row>
-    <row r="47" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A47" s="17"/>
+    <row r="47" spans="1:4" ht="25.5">
+      <c r="A47" s="16"/>
       <c r="B47" s="8" t="s">
         <v>55</v>
       </c>
@@ -1226,8 +1216,8 @@
       </c>
       <c r="D47" s="7"/>
     </row>
-    <row r="48" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A48" s="17"/>
+    <row r="48" spans="1:4" ht="25.5">
+      <c r="A48" s="16"/>
       <c r="B48" s="8" t="s">
         <v>56</v>
       </c>
@@ -1236,8 +1226,8 @@
       </c>
       <c r="D48" s="7"/>
     </row>
-    <row r="49" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A49" s="17"/>
+    <row r="49" spans="1:4" ht="38.25">
+      <c r="A49" s="16"/>
       <c r="B49" s="8" t="s">
         <v>57</v>
       </c>
@@ -1246,8 +1236,8 @@
       </c>
       <c r="D49" s="7"/>
     </row>
-    <row r="50" spans="1:4" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A50" s="14"/>
+    <row r="50" spans="1:4" ht="63.75">
+      <c r="A50" s="16"/>
       <c r="B50" s="8" t="s">
         <v>58</v>
       </c>
@@ -1256,8 +1246,8 @@
       </c>
       <c r="D50" s="7"/>
     </row>
-    <row r="51" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A51" s="14"/>
+    <row r="51" spans="1:4" ht="51">
+      <c r="A51" s="13"/>
       <c r="B51" s="8" t="s">
         <v>59</v>
       </c>
@@ -1266,8 +1256,8 @@
       </c>
       <c r="D51" s="7"/>
     </row>
-    <row r="52" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A52" s="17"/>
+    <row r="52" spans="1:4" ht="25.5">
+      <c r="A52" s="16"/>
       <c r="B52" s="8" t="s">
         <v>60</v>
       </c>
@@ -1276,8 +1266,8 @@
       </c>
       <c r="D52" s="7"/>
     </row>
-    <row r="53" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A53" s="17"/>
+    <row r="53" spans="1:4" ht="38.25">
+      <c r="A53" s="16"/>
       <c r="B53" s="8" t="s">
         <v>61</v>
       </c>
@@ -1286,8 +1276,8 @@
       </c>
       <c r="D53" s="7"/>
     </row>
-    <row r="54" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A54" s="17"/>
+    <row r="54" spans="1:4" ht="25.5">
+      <c r="A54" s="16"/>
       <c r="B54" s="8" t="s">
         <v>62</v>
       </c>
@@ -1296,7 +1286,7 @@
       </c>
       <c r="D54" s="7"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4">
       <c r="A55" s="9"/>
       <c r="B55" s="10"/>
       <c r="C55" s="11" t="s">
@@ -1318,12 +1308,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
@@ -1335,12 +1325,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
   <sheetData/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>